<commit_message>
cnn model set up
</commit_message>
<xml_diff>
--- a/Result_Quality_Log.xlsx
+++ b/Result_Quality_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carcgl-my.sharepoint.com/personal/kunyu_luo_carrier_com/Documents/Desktop/Projects/GreenShift/GreenShift_PowerPrediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{71B837C1-90ED-4137-88A7-7B05B2897D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38BF68FD-40B7-4C8A-900C-38874840E90D}"/>
+  <xr:revisionPtr revIDLastSave="360" documentId="8_{71B837C1-90ED-4137-88A7-7B05B2897D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B5872B-7A78-47BD-A026-9A13A41A6192}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2FB141B-0B76-4565-8991-7DEAB16AFBA7}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="model_1" sheetId="1" r:id="rId1"/>
     <sheet name="model_2" sheetId="2" r:id="rId2"/>
     <sheet name="model_3" sheetId="3" r:id="rId3"/>
+    <sheet name="cnn" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
   <si>
     <t>lstm unit</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -110,6 +111,30 @@
   </si>
   <si>
     <t>simply increase learning rate and number of epochs doesn't help much</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv1d filter</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernal_size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>activation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pool_size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dense</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>learning rate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -527,7 +552,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -885,14 +910,62 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="A13" s="2">
+        <v>350</v>
+      </c>
+      <c r="B13" s="2">
+        <v>150</v>
+      </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>1E-3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>12</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.28799999999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="A14" s="2">
+        <v>350</v>
+      </c>
+      <c r="B14" s="2">
+        <v>150</v>
+      </c>
+      <c r="C14">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>1E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2">
+        <v>6</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.33400000000000002</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="1"/>
@@ -930,13 +1003,14 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="13" width="9.77734375"/>
+    <col min="14" max="14" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1497,5 +1571,555 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E97A8E9-CC9B-4237-AF82-948E58EE99EF}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+      <c r="G2">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1E-3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.245</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1E-3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1E-3</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.20599999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1E-3</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1E-3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.129</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9" s="2">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>32</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.151</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>32</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>32</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13" s="2">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>32</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>32</v>
+      </c>
+      <c r="H14" s="2">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2">
+        <v>6</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
standardization; large time step test
</commit_message>
<xml_diff>
--- a/Result_Quality_Log.xlsx
+++ b/Result_Quality_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carcgl-my.sharepoint.com/personal/kunyu_luo_carrier_com/Documents/Desktop/Projects/GreenShift/GreenShift_PowerPrediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="360" documentId="8_{71B837C1-90ED-4137-88A7-7B05B2897D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B5872B-7A78-47BD-A026-9A13A41A6192}"/>
+  <xr:revisionPtr revIDLastSave="403" documentId="8_{71B837C1-90ED-4137-88A7-7B05B2897D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96EB3C20-DD74-4611-9B37-285E5FB42508}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2FB141B-0B76-4565-8991-7DEAB16AFBA7}"/>
+    <workbookView xWindow="1476" yWindow="228" windowWidth="19140" windowHeight="12000" xr2:uid="{B2FB141B-0B76-4565-8991-7DEAB16AFBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="model_1" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -232,6 +232,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1818EB1-80F4-4B71-97AE-F84A1D7AD981}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -975,21 +978,206 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="1"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>350</v>
+      </c>
+      <c r="B17" s="6">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <v>1E-3</v>
+      </c>
+      <c r="F17">
+        <v>24</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.14599999999999999</v>
+      </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>350</v>
+      </c>
+      <c r="B18" s="2">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>1E-3</v>
+      </c>
+      <c r="F18">
+        <v>24</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="J18" s="1">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>400</v>
+      </c>
+      <c r="B19" s="6">
+        <v>64</v>
+      </c>
+      <c r="C19">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>1E-3</v>
+      </c>
+      <c r="F19">
+        <v>24</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="J19" s="1">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>350</v>
+      </c>
+      <c r="B20" s="2">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>350</v>
+      </c>
+      <c r="B21" s="6">
+        <v>64</v>
+      </c>
+      <c r="C21">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2">
+        <v>70</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>24</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>350</v>
+      </c>
+      <c r="B22" s="6">
+        <v>64</v>
+      </c>
+      <c r="C22">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2">
+        <v>70</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>6</v>
+      </c>
+      <c r="G22" s="2">
+        <v>6</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>350</v>
+      </c>
+      <c r="B23" s="6">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2">
+        <v>70</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.307</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1008,9 +1196,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="13" width="9.77734375"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="13" width="12.109375"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2121,5 +2309,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>